<commit_message>
fixed bug in resulted test webscrape
</commit_message>
<xml_diff>
--- a/HL7_parsor/test.xlsx
+++ b/HL7_parsor/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,205 +466,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hepatitis B Surface Antigen (HBsAg)</t>
+          <t>Influenza Rapid</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3940036</v>
+        <v>3925638</v>
       </c>
       <c r="D2" t="n">
-        <v>11763145</v>
+        <v>32023011000653</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRESUMPTIVE POSITIVE, CONFIRMATORY TESTING PENDING</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>HEPATITIS C VIRUS (HCV) ANTIBODY</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>3939906</v>
-      </c>
-      <c r="D3" t="n">
-        <v>11752211</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Equivocal</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Hepatitis A Virus (HAV) IgM</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3939786</v>
-      </c>
-      <c r="D4" t="n">
-        <v>11734883</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Nonreactive</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>HCV LOG (LOG IU/ML)</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3939448</v>
-      </c>
-      <c r="D5" t="n">
-        <v>11730469</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>&lt; LLOQ Detected</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Hepatitis B Surface Antigen (HBsAg)</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3939418</v>
-      </c>
-      <c r="D6" t="n">
-        <v>11735717</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Nonreactive</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Hepatitis B core, IgM</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>3938626</v>
-      </c>
-      <c r="D7" t="n">
-        <v>11757000</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Nonreactive</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>HEPATITIS C (HCV) QUANTITATION (IU/mL)</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>3939491</v>
-      </c>
-      <c r="D8" t="n">
-        <v>11694625</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>116946252,888,413.004682,888,413.00L</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>HCV LOG (LOG IU/ML)</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>3939406</v>
-      </c>
-      <c r="D9" t="n">
-        <v>11725755</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2.19</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Numeric</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated code to account for issues in resulted organism field
</commit_message>
<xml_diff>
--- a/HL7_parsor/test.xlsx
+++ b/HL7_parsor/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,21 +466,203 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Influenza Rapid</t>
+          <t>Flu B PCR</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3925638</v>
+        <v>4008926</v>
       </c>
       <c r="D2" t="n">
-        <v>32023011000653</v>
+        <v>2023049001139</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Flu A PCR</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4001509</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2023046001696</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>RSV PCR</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3995090</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2023044002184</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SARSCoV2 PCR</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3994204</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2023044001487</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2 (In-house)</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3994149</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2023043001779</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Positive</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SARSCoV2 PCR</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3994135</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2023043001778</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Not Detected</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2 (In-house)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3993717</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2023044000622</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SARSCoV2 PCR</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3993716</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2023044000836</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>Categorical</t>
         </is>

</xml_diff>

<commit_message>
updated with more locators just in case id does not work
</commit_message>
<xml_diff>
--- a/HL7_parsor/test.xlsx
+++ b/HL7_parsor/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,18 +466,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Flu B PCR</t>
+          <t>Quantiferon TB Gold (Modified)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4008926</v>
+        <v>4001158</v>
       </c>
       <c r="D2" t="n">
-        <v>2023049001139</v>
+        <v>11833232</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -492,177 +492,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Flu A PCR</t>
+          <t>Quantiferon TB Gold (Modified)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4001509</v>
+        <v>4001033</v>
       </c>
       <c r="D3" t="n">
-        <v>2023046001696</v>
+        <v>11826881</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>RSV PCR</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3995090</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2023044002184</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SARSCoV2 PCR</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3994204</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2023044001487</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SARS-CoV-2 (In-house)</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3994149</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2023043001779</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SARSCoV2 PCR</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>3994135</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2023043001778</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Not Detected</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SARS-CoV-2 (In-house)</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>3993717</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2023044000622</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Categorical</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SARSCoV2 PCR</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>3993716</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2023044000836</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>NEGATIVE</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
         <is>
           <t>Categorical</t>
         </is>

</xml_diff>